<commit_message>
Updated files and added new templates
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1806" yWindow="1422" windowWidth="19266" windowHeight="6876" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -506,17 +506,13 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Not Paid</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>100</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Insta Pay</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -532,13 +528,17 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Not Paid</t>
+          <t>Paid</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="N3" t="inlineStr"/>
+        <v>1006</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Vodafone Cash</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>100</v>
+        <v>1006</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -569,17 +569,13 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Not Paid</t>
         </is>
       </c>
       <c r="L5" t="n">
-        <v>100</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="J6" t="b">

</xml_diff>

<commit_message>
Updated HTML templates and added new session files
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M1:M1048576"/>
@@ -470,6 +470,11 @@
           <t>Payment Method</t>
         </is>
       </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>2025-02-20</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -513,6 +518,9 @@
         <v>0</v>
       </c>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -524,20 +532,19 @@
         <v>1</v>
       </c>
       <c r="J3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Not Paid</t>
         </is>
       </c>
       <c r="L3" t="n">
-        <v>1006</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Vodafone Cash</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -551,16 +558,15 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Paid</t>
+          <t>Not Paid</t>
         </is>
       </c>
       <c r="L4" t="n">
-        <v>1006</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -576,6 +582,9 @@
         <v>0</v>
       </c>
       <c r="N5" t="inlineStr"/>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="J6" t="b">
@@ -590,6 +599,9 @@
         <v>0</v>
       </c>
       <c r="N6" t="inlineStr"/>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="J7" t="b">
@@ -604,6 +616,9 @@
         <v>0</v>
       </c>
       <c r="N7" t="inlineStr"/>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="J8" t="b">
@@ -618,6 +633,9 @@
         <v>0</v>
       </c>
       <c r="N8" t="inlineStr"/>
+      <c r="O8" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add some update in front and back
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M2" sqref="M1:M1048576"/>
@@ -475,6 +475,11 @@
           <t>2025-02-20</t>
         </is>
       </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>2025-04-06</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -521,6 +526,9 @@
       <c r="O2" t="b">
         <v>0</v>
       </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -546,6 +554,9 @@
       <c r="O3" t="b">
         <v>1</v>
       </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -568,6 +579,9 @@
       <c r="O4" t="b">
         <v>0</v>
       </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="J5" t="b">
@@ -585,6 +599,9 @@
       <c r="O5" t="b">
         <v>0</v>
       </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="J6" t="b">
@@ -602,6 +619,9 @@
       <c r="O6" t="b">
         <v>0</v>
       </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="J7" t="b">
@@ -619,6 +639,9 @@
       <c r="O7" t="b">
         <v>1</v>
       </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="J8" t="b">
@@ -634,6 +657,9 @@
       </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>